<commit_message>
fonction import excel ok
</commit_message>
<xml_diff>
--- a/UO.xlsx
+++ b/UO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>id</t>
   </si>
@@ -76,7 +76,7 @@
     <t>client</t>
   </si>
   <si>
-    <t>19V10008</t>
+    <t>19V10002</t>
   </si>
   <si>
     <t>19V10009</t>
@@ -88,6 +88,12 @@
     <t>19V10018</t>
   </si>
   <si>
+    <t>19V10017</t>
+  </si>
+  <si>
+    <t>19V10050</t>
+  </si>
+  <si>
     <t>SYNTH</t>
   </si>
   <si>
@@ -97,6 +103,9 @@
     <t>SYST</t>
   </si>
   <si>
+    <t>PREPA</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
@@ -172,17 +181,21 @@
     <t>SA124</t>
   </si>
   <si>
-    <t>0   2019-03-31 22:00:00+00:00
+    <t>0   2019-03-28 23:00:00+00:00
 1   2019-03-31 22:00:00+00:00
 2   2019-10-17 22:00:00+00:00
 3   2020-01-22 23:00:00+00:00
+4   2019-03-01 23:00:00+00:00
+5   2019-03-01 23:00:00+00:00
 Name: date_debut_uo, dtype: datetime64[ns, UTC]</t>
   </si>
   <si>
-    <t>0   2021-09-02 22:00:00+00:00
+    <t>0   2021-08-30 22:00:00+00:00
 1   2021-09-02 22:00:00+00:00
 2   2020-12-05 23:00:00+00:00
 3   2020-06-02 22:00:00+00:00
+4   2021-06-02 22:00:00+00:00
+5   2021-06-02 22:00:00+00:00
 Name: date_livraison, dtype: datetime64[ns, UTC]</t>
   </si>
   <si>
@@ -565,7 +578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -644,55 +657,55 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Q2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="T2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="U2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -706,55 +719,55 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="M3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="O3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Q3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="T3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="U3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -768,55 +781,55 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="P4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Q4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="T4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="U4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -830,55 +843,179 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="L5" t="s">
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" t="s">
         <v>46</v>
       </c>
-      <c r="O5" t="s">
-        <v>49</v>
-      </c>
-      <c r="P5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>52</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="N7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" t="s">
         <v>53</v>
       </c>
-      <c r="T5" t="s">
-        <v>57</v>
-      </c>
-      <c r="U5" t="s">
-        <v>61</v>
+      <c r="Q7" t="s">
+        <v>55</v>
+      </c>
+      <c r="R7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T7" t="s">
+        <v>60</v>
+      </c>
+      <c r="U7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>